<commit_message>
Mejora añadida contabilizar errores
</commit_message>
<xml_diff>
--- a/simulations/cobb_douglas_XnY1/results/hold_out_0.10/hasta_150_recopilacion_datos.xlsx
+++ b/simulations/cobb_douglas_XnY1/results/hold_out_0.10/hasta_150_recopilacion_datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Doctorado EOMA\Cafee\simulations\cobb_douglas_XnY1\results\hold_out_0.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82005779-439A-4A68-8DFD-4DB22CD57D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6064F4DC-28F4-4DCA-B8D8-696B1ADC5DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6165" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1044,6 +1044,7 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1356,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO79"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScale="87" workbookViewId="0">
-      <selection activeCell="Q47" sqref="Q47"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2149,6 +2150,10 @@
       <c r="R12" s="80">
         <v>1</v>
       </c>
+      <c r="S12" s="118">
+        <f>R12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.4">
       <c r="A13" s="40" t="s">
@@ -2204,6 +2209,10 @@
       </c>
       <c r="R13" s="82">
         <v>0</v>
+      </c>
+      <c r="S13" s="118">
+        <f>S12+R21</f>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.4">
@@ -4422,11 +4431,11 @@
         <f t="shared" si="0"/>
         <v>0.1663446748936192</v>
       </c>
-      <c r="J47" s="90">
+      <c r="J47" s="91">
         <f t="shared" si="0"/>
         <v>0.1370154072269425</v>
       </c>
-      <c r="K47" s="91">
+      <c r="K47" s="90">
         <f t="shared" si="0"/>
         <v>0.71367810935425158</v>
       </c>
@@ -4836,7 +4845,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5209,7 +5218,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:M1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5467,8 +5476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M4"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>